<commit_message>
Rename Irradiance Forcer Calculations.py to irradiance_forcing_calculations.py
</commit_message>
<xml_diff>
--- a/src/CSV Files and Plots Generated/solar_irradiance_data.xlsx
+++ b/src/CSV Files and Plots Generated/solar_irradiance_data.xlsx
@@ -477,7 +477,7 @@
         <v>2.53288867974712</v>
       </c>
       <c r="D2" t="n">
-        <v>101.3155471898848</v>
+        <v>116.5128792683675</v>
       </c>
     </row>
     <row r="3">
@@ -493,7 +493,7 @@
         <v>6.825296151564129</v>
       </c>
       <c r="D3" t="n">
-        <v>273.0118460625652</v>
+        <v>313.96362297195</v>
       </c>
     </row>
     <row r="4">
@@ -509,7 +509,7 @@
         <v>10.87628127749248</v>
       </c>
       <c r="D4" t="n">
-        <v>435.0512510996992</v>
+        <v>500.308938764654</v>
       </c>
     </row>
     <row r="5">
@@ -525,7 +525,7 @@
         <v>13.62604087812263</v>
       </c>
       <c r="D5" t="n">
-        <v>545.0416351249054</v>
+        <v>626.7978803936411</v>
       </c>
     </row>
     <row r="6">
@@ -541,7 +541,7 @@
         <v>14.95386378051026</v>
       </c>
       <c r="D6" t="n">
-        <v>598.1545512204103</v>
+        <v>687.8777339034718</v>
       </c>
     </row>
     <row r="7">
@@ -557,7 +557,7 @@
         <v>15.10117233054402</v>
       </c>
       <c r="D7" t="n">
-        <v>604.0468932217607</v>
+        <v>694.6539272050247</v>
       </c>
     </row>
     <row r="8">
@@ -573,7 +573,7 @@
         <v>14.12320723448656</v>
       </c>
       <c r="D8" t="n">
-        <v>564.9282893794626</v>
+        <v>649.667532786382</v>
       </c>
     </row>
     <row r="9">
@@ -589,7 +589,7 @@
         <v>11.47574523804652</v>
       </c>
       <c r="D9" t="n">
-        <v>459.029809521861</v>
+        <v>527.8842809501401</v>
       </c>
     </row>
     <row r="10">
@@ -605,7 +605,7 @@
         <v>7.529103668392086</v>
       </c>
       <c r="D10" t="n">
-        <v>301.1641467356834</v>
+        <v>346.338768746036</v>
       </c>
     </row>
     <row r="11">
@@ -621,7 +621,7 @@
         <v>2.895022198580109</v>
       </c>
       <c r="D11" t="n">
-        <v>115.8008879432044</v>
+        <v>133.171021134685</v>
       </c>
     </row>
     <row r="12">
@@ -637,7 +637,7 @@
         <v>0.06137856251406591</v>
       </c>
       <c r="D12" t="n">
-        <v>2.455142500562637</v>
+        <v>2.823413875647032</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>101.3155471898848</v>
+        <v>116.5128792683675</v>
       </c>
     </row>
     <row r="3">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>273.0118460625652</v>
+        <v>313.96362297195</v>
       </c>
     </row>
     <row r="4">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>435.0512510996992</v>
+        <v>500.308938764654</v>
       </c>
     </row>
     <row r="5">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>545.0416351249054</v>
+        <v>626.7978803936411</v>
       </c>
     </row>
     <row r="6">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>598.1545512204103</v>
+        <v>687.8777339034718</v>
       </c>
     </row>
     <row r="7">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>604.0468932217607</v>
+        <v>694.6539272050247</v>
       </c>
     </row>
     <row r="8">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>564.9282893794626</v>
+        <v>649.667532786382</v>
       </c>
     </row>
     <row r="9">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>459.029809521861</v>
+        <v>527.8842809501401</v>
       </c>
     </row>
     <row r="10">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>301.1641467356834</v>
+        <v>346.338768746036</v>
       </c>
     </row>
     <row r="11">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>115.8008879432044</v>
+        <v>133.171021134685</v>
       </c>
     </row>
     <row r="12">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.455142500562637</v>
+        <v>2.823413875647032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>